<commit_message>
Added rownames to table 1
</commit_message>
<xml_diff>
--- a/Export_Tables.xlsx
+++ b/Export_Tables.xlsx
@@ -10,6 +10,14 @@
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>rownames(temp)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -112,6 +120,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>-282.6592244418332</v>
+      </c>
+      <c r="C5">
+        <v>106.95441538661449</v>
+      </c>
+      <c r="D5">
+        <v>-2.6428008925118998</v>
+      </c>
+      <c r="E5">
+        <v>0.0089195273423114934</v>
+      </c>
+      <c r="F5">
+        <v>-493.65151883511487</v>
+      </c>
+      <c r="G5">
+        <v>-71.666930048551507</v>
+      </c>
+      <c r="H5">
+        <v>187</v>
+      </c>
+      <c r="I5">
+        <v>1.972731033408909</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>3054.9565217391305</v>
+      </c>
+      <c r="C6">
+        <v>66.924275134525814</v>
+      </c>
+      <c r="D6">
+        <v>45.647958317042686</v>
+      </c>
+      <c r="E6">
+        <v>2.5090064061084927e-103</v>
+      </c>
+      <c r="F6">
+        <v>2922.9329272928553</v>
+      </c>
+      <c r="G6">
+        <v>3186.9801161854057</v>
+      </c>
+      <c r="H6">
+        <v>187</v>
+      </c>
+      <c r="I6">
+        <v>1.972731033408909</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created table shell for regression 1
</commit_message>
<xml_diff>
--- a/Export_Tables.xlsx
+++ b/Export_Tables.xlsx
@@ -1,42 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Documents\StataRepro\StataReproducibility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Regression Table 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Regression Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regression Shell Table 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>rownames(temp)</t>
+  </si>
+  <si>
+    <t>Table 1. Birth weight predicted by mother's smoking during pregnancy</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>standard error</t>
+  </si>
+  <si>
+    <t>p-value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -44,25 +81,421 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10">
       <c r="A1">
         <v>-282.6592244418332</v>
       </c>
@@ -73,7 +506,7 @@
         <v>-2.6428008925118998</v>
       </c>
       <c r="D1">
-        <v>0.0089195273423114934</v>
+        <v>8.9195273423114934E-3</v>
       </c>
       <c r="E1">
         <v>-493.65151883511487</v>
@@ -91,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>3054.9565217391305</v>
       </c>
@@ -102,7 +535,7 @@
         <v>45.647958317042686</v>
       </c>
       <c r="D2">
-        <v>2.5090064061084927e-103</v>
+        <v>2.5090064061084927E-103</v>
       </c>
       <c r="E2">
         <v>2922.9329272928553</v>
@@ -120,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -134,7 +567,7 @@
         <v>-2.6428008925118998</v>
       </c>
       <c r="E5">
-        <v>0.0089195273423114934</v>
+        <v>8.9195273423114934E-3</v>
       </c>
       <c r="F5">
         <v>-493.65151883511487</v>
@@ -152,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -166,7 +599,7 @@
         <v>45.647958317042686</v>
       </c>
       <c r="E6">
-        <v>2.5090064061084927e-103</v>
+        <v>2.5090064061084927E-103</v>
       </c>
       <c r="F6">
         <v>2922.9329272928553</v>
@@ -185,5 +618,65 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exported regression shell table and added screenshots
</commit_message>
<xml_diff>
--- a/Export_Tables.xlsx
+++ b/Export_Tables.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Documents\StataRepro\StataReproducibility\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="Regression Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Regression Shell Table 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>rownames(temp)</t>
   </si>
@@ -41,12 +36,15 @@
   </si>
   <si>
     <t>p-value</t>
+  </si>
+  <si>
+    <t>12:37:34  21 Oct 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -68,7 +66,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407453"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,19 +166,19 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,7 +187,7 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill>
@@ -199,8 +197,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
+        <b val="false"/>
+        <i val="false"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -210,19 +208,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -488,14 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1">
       <c r="A1">
         <v>-282.6592244418332</v>
       </c>
@@ -524,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2">
       <c r="A2">
         <v>3054.9565217391305</v>
       </c>
@@ -553,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -585,7 +575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -623,22 +613,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="true"/>
+    <col min="2" max="2" width="14.28515625" customWidth="true"/>
+    <col min="3" max="3" width="14.5703125" customWidth="true"/>
+    <col min="4" max="4" width="15.42578125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,7 +636,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2">
       <c r="A2" s="8"/>
       <c r="B2" s="8" t="s">
         <v>4</v>
@@ -658,19 +648,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3">
+        <v>-282.6592244418332</v>
+      </c>
+      <c r="C3">
+        <v>106.95441538661449</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0089195273423114934</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="5">
+        <v>3054.9565217391305</v>
+      </c>
+      <c r="C4" s="5">
+        <v>66.924275134525814</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.5090064061084927e-103</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Created table shell for nested reg
</commit_message>
<xml_diff>
--- a/Export_Tables.xlsx
+++ b/Export_Tables.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clare\Documents\StataRepro\StataReproducibility\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regression Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Regression Shell Table 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Regression Shell Table 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>rownames(temp)</t>
   </si>
@@ -39,19 +45,61 @@
   </si>
   <si>
     <t>12:37:34  21 Oct 2018</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>s.e</t>
+  </si>
+  <si>
+    <t>s.e.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Table 2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Birthweight predicted by mother's smoking and history of hypertension</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,7 +114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407453"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,21 +212,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,7 +248,7 @@
     <dxf>
       <font>
         <b/>
-        <i val="false"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -197,8 +258,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="false"/>
-        <i val="false"/>
+        <b val="0"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -208,11 +269,19 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -478,14 +547,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10">
       <c r="A1">
         <v>-282.6592244418332</v>
       </c>
@@ -514,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>3054.9565217391305</v>
       </c>
@@ -543,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -575,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -613,43 +682,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="true"/>
-    <col min="2" max="2" width="14.28515625" customWidth="true"/>
-    <col min="3" max="3" width="14.5703125" customWidth="true"/>
-    <col min="4" max="4" width="15.42578125" customWidth="true"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -658,25 +727,25 @@
       <c r="C3">
         <v>106.95441538661449</v>
       </c>
-      <c r="D3" s="3">
-        <v>0.0089195273423114934</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="2">
+        <v>8.9195273423114934E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3054.9565217391305</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>66.924275134525814</v>
       </c>
-      <c r="D4" s="4">
-        <v>2.5090064061084927e-103</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="D4" s="3">
+        <v>2.5090064061084927E-103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -688,4 +757,159 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4"/>
+      <c r="B3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed nested code to remove constant
</commit_message>
<xml_diff>
--- a/Export_Tables.xlsx
+++ b/Export_Tables.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>rownames(temp)</t>
   </si>
@@ -79,6 +79,9 @@
       </rPr>
       <t xml:space="preserve"> Birthweight predicted by mother's smoking and history of hypertension</t>
     </r>
+  </si>
+  <si>
+    <t>09:33:55 29 Oct 2018</t>
   </si>
 </sst>
 </file>
@@ -221,6 +224,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,16 +240,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,12 +701,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6"/>
@@ -761,10 +764,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,135 +776,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="11">
+        <v>-282.6592244418332</v>
+      </c>
+      <c r="C4" s="11">
+        <v>106.95441538661449</v>
+      </c>
+      <c r="D4" s="12">
+        <v>8.9195273423114934E-3</v>
+      </c>
+      <c r="E4" s="11">
+        <v>-279.79477928026864</v>
+      </c>
+      <c r="F4" s="11">
+        <v>106.10089612312176</v>
+      </c>
+      <c r="G4" s="12">
+        <v>9.0700351530636873E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11">
+        <v>-427.65663727920224</v>
+      </c>
+      <c r="F5" s="11">
+        <v>212.37655697328654</v>
+      </c>
+      <c r="G5" s="12">
+        <v>4.5485224750764136E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
+      <c r="A14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>